<commit_message>
- results thomas added to skydiver_everyone.xlsx
</commit_message>
<xml_diff>
--- a/benchmark_opdracht/results/skydiver_everyone.xlsx
+++ b/benchmark_opdracht/results/skydiver_everyone.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Brian" sheetId="1" r:id="rId1"/>
     <sheet name="Dieter" sheetId="2" r:id="rId2"/>
+    <sheet name="Thomas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>gfx_1_FPS</t>
   </si>
@@ -253,6 +254,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -280,7 +282,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -566,19 +567,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1035,7 +1037,7 @@
       <c r="L13">
         <v>21279</v>
       </c>
-      <c r="M13" s="13"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14">
@@ -1728,19 +1730,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1812,11 +1815,11 @@
       <c r="L2">
         <v>5204</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3">
@@ -1852,9 +1855,9 @@
       <c r="L3">
         <v>5219</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4">
@@ -1890,9 +1893,9 @@
       <c r="L4">
         <v>5210</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="9"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1928,9 +1931,9 @@
       <c r="L5">
         <v>5218</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="12"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6">
@@ -2899,4 +2902,1129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>26.048376083373999</v>
+      </c>
+      <c r="C2">
+        <v>25.862993240356399</v>
+      </c>
+      <c r="D2">
+        <v>25.3418292999268</v>
+      </c>
+      <c r="E2">
+        <v>93.516754150390597</v>
+      </c>
+      <c r="F2">
+        <v>67.967353820800795</v>
+      </c>
+      <c r="G2">
+        <v>43.583847045898402</v>
+      </c>
+      <c r="H2">
+        <v>24.9743843078613</v>
+      </c>
+      <c r="I2">
+        <v>5684</v>
+      </c>
+      <c r="J2">
+        <v>7431</v>
+      </c>
+      <c r="K2">
+        <v>6158</v>
+      </c>
+      <c r="L2">
+        <v>5939</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>26.046510696411101</v>
+      </c>
+      <c r="C3">
+        <v>25.797910690307599</v>
+      </c>
+      <c r="D3">
+        <v>25.328229904174801</v>
+      </c>
+      <c r="E3">
+        <v>104.27025604248</v>
+      </c>
+      <c r="F3">
+        <v>71.893760681152301</v>
+      </c>
+      <c r="G3">
+        <v>43.9293022155762</v>
+      </c>
+      <c r="H3">
+        <v>24.337133407592798</v>
+      </c>
+      <c r="I3">
+        <v>5676</v>
+      </c>
+      <c r="J3">
+        <v>7242</v>
+      </c>
+      <c r="K3">
+        <v>6154</v>
+      </c>
+      <c r="L3">
+        <v>5913</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>26.060497283935501</v>
+      </c>
+      <c r="C4">
+        <v>25.802526473998999</v>
+      </c>
+      <c r="D4">
+        <v>25.355442047119102</v>
+      </c>
+      <c r="E4">
+        <v>92.720077514648395</v>
+      </c>
+      <c r="F4">
+        <v>61.628948211669901</v>
+      </c>
+      <c r="G4">
+        <v>41.271469116210902</v>
+      </c>
+      <c r="H4">
+        <v>23.897764205932599</v>
+      </c>
+      <c r="I4">
+        <v>5678</v>
+      </c>
+      <c r="J4">
+        <v>7111</v>
+      </c>
+      <c r="K4">
+        <v>6161</v>
+      </c>
+      <c r="L4">
+        <v>5902</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>26.0776252746582</v>
+      </c>
+      <c r="C5">
+        <v>25.837388992309599</v>
+      </c>
+      <c r="D5">
+        <v>25.3839817047119</v>
+      </c>
+      <c r="E5">
+        <v>103.554191589355</v>
+      </c>
+      <c r="F5">
+        <v>69.559669494628906</v>
+      </c>
+      <c r="G5">
+        <v>42.7404975891113</v>
+      </c>
+      <c r="H5">
+        <v>23.696681976318398</v>
+      </c>
+      <c r="I5">
+        <v>5684</v>
+      </c>
+      <c r="J5">
+        <v>7051</v>
+      </c>
+      <c r="K5">
+        <v>6168</v>
+      </c>
+      <c r="L5">
+        <v>5901</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>26.055833816528299</v>
+      </c>
+      <c r="C6">
+        <v>25.768583297729499</v>
+      </c>
+      <c r="D6">
+        <v>25.380348205566399</v>
+      </c>
+      <c r="E6">
+        <v>101.024894714355</v>
+      </c>
+      <c r="F6">
+        <v>69.181587219238295</v>
+      </c>
+      <c r="G6">
+        <v>42.520492553710902</v>
+      </c>
+      <c r="H6">
+        <v>23.6633415222168</v>
+      </c>
+      <c r="I6">
+        <v>5674</v>
+      </c>
+      <c r="J6">
+        <v>7041</v>
+      </c>
+      <c r="K6">
+        <v>6167</v>
+      </c>
+      <c r="L6">
+        <v>5892</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>26.068895339965799</v>
+      </c>
+      <c r="C7">
+        <v>25.791450500488299</v>
+      </c>
+      <c r="D7">
+        <v>25.3685417175293</v>
+      </c>
+      <c r="E7">
+        <v>104.416496276855</v>
+      </c>
+      <c r="F7">
+        <v>69.731803894042997</v>
+      </c>
+      <c r="G7">
+        <v>43.023105621337898</v>
+      </c>
+      <c r="H7">
+        <v>23.745691299438501</v>
+      </c>
+      <c r="I7">
+        <v>5678</v>
+      </c>
+      <c r="J7">
+        <v>7066</v>
+      </c>
+      <c r="K7">
+        <v>6164</v>
+      </c>
+      <c r="L7">
+        <v>5898</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>26.0502414703369</v>
+      </c>
+      <c r="C8">
+        <v>25.793296813964801</v>
+      </c>
+      <c r="D8">
+        <v>25.344551086425799</v>
+      </c>
+      <c r="E8">
+        <v>101.637908935547</v>
+      </c>
+      <c r="F8">
+        <v>71.218887329101605</v>
+      </c>
+      <c r="G8">
+        <v>42.827922821044901</v>
+      </c>
+      <c r="H8">
+        <v>23.7088298797607</v>
+      </c>
+      <c r="I8">
+        <v>5676</v>
+      </c>
+      <c r="J8">
+        <v>7055</v>
+      </c>
+      <c r="K8">
+        <v>6158</v>
+      </c>
+      <c r="L8">
+        <v>5894</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>26.062362670898398</v>
+      </c>
+      <c r="C9">
+        <v>25.874099731445298</v>
+      </c>
+      <c r="D9">
+        <v>25.356746673583999</v>
+      </c>
+      <c r="E9">
+        <v>106.193397521973</v>
+      </c>
+      <c r="F9">
+        <v>68.662422180175795</v>
+      </c>
+      <c r="G9">
+        <v>42.093143463134801</v>
+      </c>
+      <c r="H9">
+        <v>23.897764205932599</v>
+      </c>
+      <c r="I9">
+        <v>5686</v>
+      </c>
+      <c r="J9">
+        <v>7111</v>
+      </c>
+      <c r="K9">
+        <v>6161</v>
+      </c>
+      <c r="L9">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>26.0493068695068</v>
+      </c>
+      <c r="C10">
+        <v>25.798833847045898</v>
+      </c>
+      <c r="D10">
+        <v>25.383073806762699</v>
+      </c>
+      <c r="E10">
+        <v>104.486335754395</v>
+      </c>
+      <c r="F10">
+        <v>64.853820800781307</v>
+      </c>
+      <c r="G10">
+        <v>42.349029541015597</v>
+      </c>
+      <c r="H10">
+        <v>24.096385955810501</v>
+      </c>
+      <c r="I10">
+        <v>5677</v>
+      </c>
+      <c r="J10">
+        <v>7170</v>
+      </c>
+      <c r="K10">
+        <v>6168</v>
+      </c>
+      <c r="L10">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>26.0502414703369</v>
+      </c>
+      <c r="C11">
+        <v>25.840162277221701</v>
+      </c>
+      <c r="D11">
+        <v>25.296075820922901</v>
+      </c>
+      <c r="E11">
+        <v>104.20929718017599</v>
+      </c>
+      <c r="F11">
+        <v>68.248497009277301</v>
+      </c>
+      <c r="G11">
+        <v>42.2697563171387</v>
+      </c>
+      <c r="H11">
+        <v>23.971284866333001</v>
+      </c>
+      <c r="I11">
+        <v>5681</v>
+      </c>
+      <c r="J11">
+        <v>7133</v>
+      </c>
+      <c r="K11">
+        <v>6146</v>
+      </c>
+      <c r="L11">
+        <v>5906</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>26.0549011230469</v>
+      </c>
+      <c r="C12">
+        <v>25.763801574706999</v>
+      </c>
+      <c r="D12">
+        <v>25.3536262512207</v>
+      </c>
+      <c r="E12">
+        <v>105.11695861816401</v>
+      </c>
+      <c r="F12">
+        <v>69.251373291015597</v>
+      </c>
+      <c r="G12">
+        <v>41.890167236328097</v>
+      </c>
+      <c r="H12">
+        <v>23.909986495971701</v>
+      </c>
+      <c r="I12">
+        <v>5673</v>
+      </c>
+      <c r="J12">
+        <v>7115</v>
+      </c>
+      <c r="K12">
+        <v>6160</v>
+      </c>
+      <c r="L12">
+        <v>5898</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>26.038681030273398</v>
+      </c>
+      <c r="C13">
+        <v>25.798833847045898</v>
+      </c>
+      <c r="D13">
+        <v>25.325977325439499</v>
+      </c>
+      <c r="E13">
+        <v>101.47682189941401</v>
+      </c>
+      <c r="F13">
+        <v>70.363288879394503</v>
+      </c>
+      <c r="G13">
+        <v>42.732856750488303</v>
+      </c>
+      <c r="H13">
+        <v>23.8003845214844</v>
+      </c>
+      <c r="I13">
+        <v>5676</v>
+      </c>
+      <c r="J13">
+        <v>7082</v>
+      </c>
+      <c r="K13">
+        <v>6154</v>
+      </c>
+      <c r="L13">
+        <v>5897</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>26.0521030426025</v>
+      </c>
+      <c r="C14">
+        <v>25.842014312744102</v>
+      </c>
+      <c r="D14">
+        <v>25.327323913574201</v>
+      </c>
+      <c r="E14">
+        <v>105.994148254395</v>
+      </c>
+      <c r="F14">
+        <v>69.871223449707003</v>
+      </c>
+      <c r="G14">
+        <v>42.4715385437012</v>
+      </c>
+      <c r="H14">
+        <v>24.047071456909201</v>
+      </c>
+      <c r="I14">
+        <v>5682</v>
+      </c>
+      <c r="J14">
+        <v>7156</v>
+      </c>
+      <c r="K14">
+        <v>6154</v>
+      </c>
+      <c r="L14">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>26.055833816528299</v>
+      </c>
+      <c r="C15">
+        <v>25.807144165039102</v>
+      </c>
+      <c r="D15">
+        <v>25.332328796386701</v>
+      </c>
+      <c r="E15">
+        <v>105.985404968262</v>
+      </c>
+      <c r="F15">
+        <v>72.239952087402301</v>
+      </c>
+      <c r="G15">
+        <v>43.389484405517599</v>
+      </c>
+      <c r="H15">
+        <v>23.8492126464844</v>
+      </c>
+      <c r="I15">
+        <v>5678</v>
+      </c>
+      <c r="J15">
+        <v>7097</v>
+      </c>
+      <c r="K15">
+        <v>6155</v>
+      </c>
+      <c r="L15">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>26.053970336914102</v>
+      </c>
+      <c r="C16">
+        <v>25.817308425903299</v>
+      </c>
+      <c r="D16">
+        <v>25.359073638916001</v>
+      </c>
+      <c r="E16">
+        <v>103.39280700683599</v>
+      </c>
+      <c r="F16">
+        <v>69.322097778320298</v>
+      </c>
+      <c r="G16">
+        <v>42.177913665771499</v>
+      </c>
+      <c r="H16">
+        <v>24.071702957153299</v>
+      </c>
+      <c r="I16">
+        <v>5679</v>
+      </c>
+      <c r="J16">
+        <v>7163</v>
+      </c>
+      <c r="K16">
+        <v>6162</v>
+      </c>
+      <c r="L16">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>26.048376083373999</v>
+      </c>
+      <c r="C17">
+        <v>25.846637725830099</v>
+      </c>
+      <c r="D17">
+        <v>25.289251327514599</v>
+      </c>
+      <c r="E17">
+        <v>101.551063537598</v>
+      </c>
+      <c r="F17">
+        <v>70.499748229980497</v>
+      </c>
+      <c r="G17">
+        <v>42.906398773193402</v>
+      </c>
+      <c r="H17">
+        <v>24.059379577636701</v>
+      </c>
+      <c r="I17">
+        <v>5682</v>
+      </c>
+      <c r="J17">
+        <v>7159</v>
+      </c>
+      <c r="K17">
+        <v>6145</v>
+      </c>
+      <c r="L17">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>26.058631896972699</v>
+      </c>
+      <c r="C18">
+        <v>25.869472503662099</v>
+      </c>
+      <c r="D18">
+        <v>25.293779373168899</v>
+      </c>
+      <c r="E18">
+        <v>103.67990875244099</v>
+      </c>
+      <c r="F18">
+        <v>68.596199035644503</v>
+      </c>
+      <c r="G18">
+        <v>42.219387054443402</v>
+      </c>
+      <c r="H18">
+        <v>23.8675727844238</v>
+      </c>
+      <c r="I18">
+        <v>5686</v>
+      </c>
+      <c r="J18">
+        <v>7102</v>
+      </c>
+      <c r="K18">
+        <v>6146</v>
+      </c>
+      <c r="L18">
+        <v>5906</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>26.061429977416999</v>
+      </c>
+      <c r="C19">
+        <v>25.877805709838899</v>
+      </c>
+      <c r="D19">
+        <v>25.320981979370099</v>
+      </c>
+      <c r="E19">
+        <v>102.25277709960901</v>
+      </c>
+      <c r="F19">
+        <v>69.595199584960895</v>
+      </c>
+      <c r="G19">
+        <v>42.873550415039098</v>
+      </c>
+      <c r="H19">
+        <v>23.377618789672901</v>
+      </c>
+      <c r="I19">
+        <v>5687</v>
+      </c>
+      <c r="J19">
+        <v>6956</v>
+      </c>
+      <c r="K19">
+        <v>6152</v>
+      </c>
+      <c r="L19">
+        <v>5892</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>26.039058685302699</v>
+      </c>
+      <c r="C20">
+        <v>25.841087341308601</v>
+      </c>
+      <c r="D20">
+        <v>25.309658050537099</v>
+      </c>
+      <c r="E20">
+        <v>102.95408630371099</v>
+      </c>
+      <c r="F20">
+        <v>70.296524047851605</v>
+      </c>
+      <c r="G20">
+        <v>42.78759765625</v>
+      </c>
+      <c r="H20">
+        <v>23.824771881103501</v>
+      </c>
+      <c r="I20">
+        <v>5680</v>
+      </c>
+      <c r="J20">
+        <v>7089</v>
+      </c>
+      <c r="K20">
+        <v>6150</v>
+      </c>
+      <c r="L20">
+        <v>5901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>26.053035736083999</v>
+      </c>
+      <c r="C21">
+        <v>25.878400802612301</v>
+      </c>
+      <c r="D21">
+        <v>25.305130004882798</v>
+      </c>
+      <c r="E21">
+        <v>102.076629638672</v>
+      </c>
+      <c r="F21">
+        <v>71.510665893554702</v>
+      </c>
+      <c r="G21">
+        <v>42.754737854003899</v>
+      </c>
+      <c r="H21">
+        <v>23.653427124023398</v>
+      </c>
+      <c r="I21">
+        <v>5686</v>
+      </c>
+      <c r="J21">
+        <v>7038</v>
+      </c>
+      <c r="K21">
+        <v>6149</v>
+      </c>
+      <c r="L21">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>26.0321559906006</v>
+      </c>
+      <c r="C22">
+        <v>25.861143112182599</v>
+      </c>
+      <c r="D22">
+        <v>25.316001892089801</v>
+      </c>
+      <c r="E22">
+        <v>101.771858215332</v>
+      </c>
+      <c r="F22">
+        <v>70.370368957519503</v>
+      </c>
+      <c r="G22">
+        <v>42.547737121582003</v>
+      </c>
+      <c r="H22">
+        <v>23.8583889007568</v>
+      </c>
+      <c r="I22">
+        <v>5682</v>
+      </c>
+      <c r="J22">
+        <v>7099</v>
+      </c>
+      <c r="K22">
+        <v>6151</v>
+      </c>
+      <c r="L22">
+        <v>5903</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>26.0349521636963</v>
+      </c>
+      <c r="C23">
+        <v>25.837388992309599</v>
+      </c>
+      <c r="D23">
+        <v>25.3536262512207</v>
+      </c>
+      <c r="E23">
+        <v>100.75934600830099</v>
+      </c>
+      <c r="F23">
+        <v>68.961120605468807</v>
+      </c>
+      <c r="G23">
+        <v>42.384780883789098</v>
+      </c>
+      <c r="H23">
+        <v>24.087123870849599</v>
+      </c>
+      <c r="I23">
+        <v>5679</v>
+      </c>
+      <c r="J23">
+        <v>7167</v>
+      </c>
+      <c r="K23">
+        <v>6160</v>
+      </c>
+      <c r="L23">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>26.0521030426025</v>
+      </c>
+      <c r="C24">
+        <v>25.871324539184599</v>
+      </c>
+      <c r="D24">
+        <v>25.348178863525401</v>
+      </c>
+      <c r="E24">
+        <v>98.420593261718807</v>
+      </c>
+      <c r="F24">
+        <v>65.663650512695298</v>
+      </c>
+      <c r="G24">
+        <v>41.810508728027301</v>
+      </c>
+      <c r="H24">
+        <v>23.891656875610401</v>
+      </c>
+      <c r="I24">
+        <v>5685</v>
+      </c>
+      <c r="J24">
+        <v>7109</v>
+      </c>
+      <c r="K24">
+        <v>6159</v>
+      </c>
+      <c r="L24">
+        <v>5907</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>26.046510696411101</v>
+      </c>
+      <c r="C25">
+        <v>25.8454265594482</v>
+      </c>
+      <c r="D25">
+        <v>25.332761764526399</v>
+      </c>
+      <c r="E25">
+        <v>105.940879821777</v>
+      </c>
+      <c r="F25">
+        <v>69.392974853515597</v>
+      </c>
+      <c r="G25">
+        <v>42.0985298156738</v>
+      </c>
+      <c r="H25">
+        <v>23.919160842895501</v>
+      </c>
+      <c r="I25">
+        <v>5682</v>
+      </c>
+      <c r="J25">
+        <v>7117</v>
+      </c>
+      <c r="K25">
+        <v>6155</v>
+      </c>
+      <c r="L25">
+        <v>5906</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>26.039058685302699</v>
+      </c>
+      <c r="C26">
+        <v>25.884290695190401</v>
+      </c>
+      <c r="D26">
+        <v>25.296554565429702</v>
+      </c>
+      <c r="E26">
+        <v>104.410049438477</v>
+      </c>
+      <c r="F26">
+        <v>68.622444152832003</v>
+      </c>
+      <c r="G26">
+        <v>42.438961029052699</v>
+      </c>
+      <c r="H26">
+        <v>24.100994110107401</v>
+      </c>
+      <c r="I26">
+        <v>5685</v>
+      </c>
+      <c r="J26">
+        <v>7172</v>
+      </c>
+      <c r="K26">
+        <v>6147</v>
+      </c>
+      <c r="L26">
+        <v>5913</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>26.040922164916999</v>
+      </c>
+      <c r="C27">
+        <v>25.868547439575199</v>
+      </c>
+      <c r="D27">
+        <v>25.2879314422607</v>
+      </c>
+      <c r="E27">
+        <v>105.755180358887</v>
+      </c>
+      <c r="F27">
+        <v>69.256324768066406</v>
+      </c>
+      <c r="G27">
+        <v>42.504161834716797</v>
+      </c>
+      <c r="H27">
+        <v>24.059379577636701</v>
+      </c>
+      <c r="I27">
+        <v>5684</v>
+      </c>
+      <c r="J27">
+        <v>7159</v>
+      </c>
+      <c r="K27">
+        <v>6144</v>
+      </c>
+      <c r="L27">
+        <v>5910</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>26.053970336914102</v>
+      </c>
+      <c r="C28">
+        <v>25.862993240356399</v>
+      </c>
+      <c r="D28">
+        <v>25.331855773925799</v>
+      </c>
+      <c r="E28">
+        <v>103.14557647705099</v>
+      </c>
+      <c r="F28">
+        <v>69.669517517089801</v>
+      </c>
+      <c r="G28">
+        <v>42.667346954345703</v>
+      </c>
+      <c r="H28">
+        <v>24.028629302978501</v>
+      </c>
+      <c r="I28">
+        <v>5684</v>
+      </c>
+      <c r="J28">
+        <v>7150</v>
+      </c>
+      <c r="K28">
+        <v>6155</v>
+      </c>
+      <c r="L28">
+        <v>5911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>26.035333633422901</v>
+      </c>
+      <c r="C29">
+        <v>25.852821350097699</v>
+      </c>
+      <c r="D29">
+        <v>25.305130004882798</v>
+      </c>
+      <c r="E29">
+        <v>104.455810546875</v>
+      </c>
+      <c r="F29">
+        <v>69.417907714843807</v>
+      </c>
+      <c r="G29">
+        <v>42.716461181640597</v>
+      </c>
+      <c r="H29">
+        <v>23.550491333007798</v>
+      </c>
+      <c r="I29">
+        <v>5681</v>
+      </c>
+      <c r="J29">
+        <v>7008</v>
+      </c>
+      <c r="K29">
+        <v>6149</v>
+      </c>
+      <c r="L29">
+        <v>5893</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>26.045579910278299</v>
+      </c>
+      <c r="C30">
+        <v>25.838312149047901</v>
+      </c>
+      <c r="D30">
+        <v>25.331855773925799</v>
+      </c>
+      <c r="E30">
+        <v>101.56364440918</v>
+      </c>
+      <c r="F30">
+        <v>69.511878967285199</v>
+      </c>
+      <c r="G30">
+        <v>42.8060302734375</v>
+      </c>
+      <c r="H30">
+        <v>24.059379577636701</v>
+      </c>
+      <c r="I30">
+        <v>5681</v>
+      </c>
+      <c r="J30">
+        <v>7159</v>
+      </c>
+      <c r="K30">
+        <v>6155</v>
+      </c>
+      <c r="L30">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1">
+        <f>AVERAGE(B1:B30)</f>
+        <v>26.050568942365967</v>
+      </c>
+      <c r="C31" s="1">
+        <f>AVERAGE(C1:C30)</f>
+        <v>25.835586218998348</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" ref="D31:L31" si="0">AVERAGE(D1:D30)</f>
+        <v>25.333098181362811</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>102.64597083782327</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>69.150317619586815</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>42.578852291764882</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>23.931227388053095</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>5680.8965517241377</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>7120.9655172413795</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>6155.4137931034484</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>5904.9310344827591</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mijn gegevens pc toegevoegd
</commit_message>
<xml_diff>
--- a/benchmark_opdracht/results/skydiver_everyone.xlsx
+++ b/benchmark_opdracht/results/skydiver_everyone.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Onderzoekstechnieken\ozt-2a1\benchmark_opdracht\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diete\Desktop\OZT Repo Brain\benchmark_opdracht\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,12 @@
     <sheet name="Dieter" sheetId="2" r:id="rId5"/>
     <sheet name="Thomas" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
   <si>
     <t>gfx_1_FPS</t>
   </si>
@@ -136,11 +136,32 @@
   <si>
     <t>1600 MHz</t>
   </si>
+  <si>
+    <t>NVIDIA GeForce 840M</t>
+  </si>
+  <si>
+    <t>1029 MHz</t>
+  </si>
+  <si>
+    <t>2048 MB</t>
+  </si>
+  <si>
+    <t>900 MHz</t>
+  </si>
+  <si>
+    <t>Intel® Core™ i7-4510U</t>
+  </si>
+  <si>
+    <t>2 (4 virtual)</t>
+  </si>
+  <si>
+    <t>2,00GHz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -359,10 +380,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Linked Cell" xfId="3" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Gekoppelde cel" xfId="3" builtinId="24"/>
+    <cellStyle name="Kop 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,9 +399,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -418,7 +439,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -490,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,7 +877,7 @@
   <dimension ref="A2:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -960,16 +981,36 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
voorbeeld charts + comments
</commit_message>
<xml_diff>
--- a/benchmark_opdracht/results/skydiver_everyone.xlsx
+++ b/benchmark_opdracht/results/skydiver_everyone.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diete\Desktop\OZT Repo Brain\benchmark_opdracht\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Onderzoekstechnieken\ozt-2a1\benchmark_opdracht\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="870" windowWidth="14940" windowHeight="9150" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="870" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="5" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Dieter" sheetId="2" r:id="rId5"/>
     <sheet name="Thomas" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>gfx_1_FPS</t>
   </si>
@@ -157,12 +157,54 @@
   <si>
     <t>2,00GHz</t>
   </si>
+  <si>
+    <t>Grafische test #1</t>
+  </si>
+  <si>
+    <t>Grafische test #2</t>
+  </si>
+  <si>
+    <t>physics level 1</t>
+  </si>
+  <si>
+    <t>physics level 2</t>
+  </si>
+  <si>
+    <t>physics level 3</t>
+  </si>
+  <si>
+    <t>physics level 4</t>
+  </si>
+  <si>
+    <t>Scores als aparte tabellen bekijken</t>
+  </si>
+  <si>
+    <t>Grafisch ver uit elkaar door uitschieter</t>
+  </si>
+  <si>
+    <t>Physics dichter bij elkaar (CPU ? Conclusie ?)</t>
+  </si>
+  <si>
+    <t>Physics mss aparte charts ?</t>
+  </si>
+  <si>
+    <t>duidelijk groot verschil level 1</t>
+  </si>
+  <si>
+    <t>heel klein verschil level 4</t>
+  </si>
+  <si>
+    <t>uitleg over threshold bij Dieter (- value)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -200,6 +242,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -337,13 +383,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
@@ -378,12 +425,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
-    <cellStyle name="Gekoppelde cel" xfId="3" builtinId="24"/>
-    <cellStyle name="Kop 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Linked Cell" xfId="3" builtinId="24"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,10 +448,2328 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Grafische testen</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Grafische test #1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grafische test #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>140.49131113688148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143.59728927612304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jovi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Grafische test #1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grafische test #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$3:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29.730401166280114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.831189219156897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Grafische test #1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grafische test #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.543362744649247</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.396382586161295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thomas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Grafische test #1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grafische test #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>26.050568942365967</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.835586218998348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-632475888"/>
+        <c:axId val="-632469904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-632475888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-632469904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-632469904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="160"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800"/>
+                  <a:t>Gemiddelde frames per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-632475888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="20"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Physics</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Test</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$E$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>physics level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>physics level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>physics level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>physics level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$E$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>155.71141001383467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.552268473307294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.188769149780271</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.07075068155924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jovi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$E$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>physics level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>physics level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>physics level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>physics level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>59.124338150024407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.458816909790038</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.244485092163096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.811899884541837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$E$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>physics level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>physics level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>physics level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>physics level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>70.965247090657556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.70590273539225</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.043619537353514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thomas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$E$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>physics level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>physics level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>physics level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>physics level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>102.64597083782327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.150317619586815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.578852291764882</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.931227388053095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-529891440"/>
+        <c:axId val="-529884912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-529891440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-529884912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-529884912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Gemiddelde frames per second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="800">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-529891440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>614362</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -439,7 +2807,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -511,7 +2879,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -661,45 +3029,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -714,161 +3083,192 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="14">
         <v>140.49131113688148</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="14">
         <v>143.59728927612304</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="14">
         <v>72.324103291829431</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="14">
         <v>155.71141001383467</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="14">
         <v>89.552268473307294</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="14">
         <v>51.188769149780271</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="14">
         <v>28.07075068155924</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="14">
         <v>31062.3</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="14">
         <v>8352.8333333333339</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="14">
         <v>17574.3</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="14">
         <v>20913.266666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="14">
         <v>29.730401166280114</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="14">
         <v>28.831189219156897</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="14">
         <v>26.682548014322922</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="14">
         <v>59.124338150024407</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="14">
         <v>59.458816909790038</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="14">
         <v>44.244485092163096</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="14">
         <v>25.811899884541837</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="14">
         <v>6410.166666666667</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="14">
         <v>7679.4333333333334</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="14">
         <v>6483.2666666666664</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="14">
         <v>6574.9333333333334</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="14">
         <v>25.543362744649247</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="14">
         <v>24.396382586161295</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="14">
         <v>25.000176620483405</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="14">
         <v>70.965247090657556</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="14">
         <v>40.70590273539225</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="14">
         <v>23.043619537353514</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="14">
         <v>5464.9666666666662</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="14">
         <v>3940.0333333333333</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="14">
         <v>6074.5666666666666</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="14">
         <v>5214</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="14">
         <v>26.050568942365967</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="14">
         <v>25.835586218998348</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="14">
         <v>25.333098181362811</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="14">
         <v>102.64597083782327</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="14">
         <v>69.150317619586815</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="14">
         <v>42.578852291764882</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="14">
         <v>23.931227388053095</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="14">
         <v>5680.8965517241377</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="14">
         <v>7120.9655172413795</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="14">
         <v>6155.4137931034484</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="14">
         <v>5904.9310344827591</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="N5" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N13" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N14" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N15" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -876,7 +3276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
zou hopelijk goed genoeg moeten zijn
</commit_message>
<xml_diff>
--- a/benchmark_opdracht/results/skydiver_everyone.xlsx
+++ b/benchmark_opdracht/results/skydiver_everyone.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="1470" windowWidth="14940" windowHeight="9150"/>
+    <workbookView xWindow="360" yWindow="2070" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="5" r:id="rId1"/>
@@ -812,11 +812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="518766784"/>
-        <c:axId val="518768352"/>
+        <c:axId val="231959080"/>
+        <c:axId val="231957120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="518766784"/>
+        <c:axId val="231959080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,7 +859,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518768352"/>
+        <c:crossAx val="231957120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -867,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="518768352"/>
+        <c:axId val="231957120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -985,7 +985,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518766784"/>
+        <c:crossAx val="231959080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -1449,11 +1449,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="520171960"/>
-        <c:axId val="520171568"/>
+        <c:axId val="231954376"/>
+        <c:axId val="231954768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="520171960"/>
+        <c:axId val="231954376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,7 +1496,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520171568"/>
+        <c:crossAx val="231954768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1504,7 +1504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520171568"/>
+        <c:axId val="231954768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="165"/>
@@ -1624,7 +1624,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520171960"/>
+        <c:crossAx val="231954376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -1713,6 +1713,799 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Algemene Scores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MSI GT72</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gfx_score</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>phsyics_score</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>combined_score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>overall_score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$I$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31062.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8352.8333333333339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17574.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20913.266666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MSI GE60</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gfx_score</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>phsyics_score</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>combined_score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>overall_score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$I$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6410.166666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7679.4333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6483.2666666666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6574.9333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Acer Aspire E17</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gfx_score</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>phsyics_score</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>combined_score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>overall_score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$I$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5464.9666666666662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3940.0333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6074.5666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Aspire V3 772G</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$I$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gfx_score</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>phsyics_score</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>combined_score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>overall_score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$I$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5680.8965517241377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7120.9655172413795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6155.4137931034484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5904.9310344827591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="423075480"/>
+        <c:axId val="423078224"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$I$1:$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>gfx_score</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>phsyics_score</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>combined_score</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>overall_score</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$I$1:$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>gfx_score</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>phsyics_score</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>combined_score</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>overall_score</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$I$1:$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>gfx_score</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>phsyics_score</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>combined_score</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>overall_score</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$I$1:$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>gfx_score</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>phsyics_score</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>combined_score</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>overall_score</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Main!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="423075480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423078224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="423078224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423075480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1754,6 +2547,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2799,6 +3632,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2856,6 +4192,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3130,7 +4496,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>